<commit_message>
laba2 + excel formula
</commit_message>
<xml_diff>
--- a/ServletStud/src/main/webapp/resources/dictionary.xlsx
+++ b/ServletStud/src/main/webapp/resources/dictionary.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\java\aiprp\lab2\ServletStud\src\main\webapp\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951F9CE6-00A8-4778-AF27-6B9C0AEC379D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3DBDC25-0A4C-4E39-B632-9D9E33D1B129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3024" yWindow="1848" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -530,7 +530,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -540,6 +540,12 @@
         <v>14</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <f>SUM(1,2)</f>
+        <v>3</v>
+      </c>
+    </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F16" t="s">
         <v>15</v>

</xml_diff>